<commit_message>
test import company and account company
</commit_message>
<xml_diff>
--- a/public/exports/sub_constructor_accounts.xlsx
+++ b/public/exports/sub_constructor_accounts.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhnt/Code/PBVN-Projects/cag-backpack/public/exports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/cag-backpack/public/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BAFECD-5337-E54D-A0BA-A90A2F9E2B91}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="37660" windowHeight="21140" xr2:uid="{B3C51E56-BDFA-9C4D-93DB-F277C8937142}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="37660" windowHeight="20000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -66,13 +68,13 @@
     <t>Sub-Name3</t>
   </si>
   <si>
-    <t>3214</t>
+    <t>12323</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -431,11 +433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409DEACB-94A0-5A4A-8D8A-4C2AE2787E8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,9 +505,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{705A7D33-866F-4346-BD98-DEBB4D603E1E}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{67F71573-4071-E34A-AC4A-F76431CF4581}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{36555CFA-1FA9-6F48-A33F-6596A01C2794}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix login user upload, add role user upload
</commit_message>
<xml_diff>
--- a/public/exports/sub_constructor_accounts.xlsx
+++ b/public/exports/sub_constructor_accounts.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Company Code</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>company coordinator</t>
+  </si>
+  <si>
+    <t>company as</t>
+  </si>
+  <si>
+    <t>company viewer</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,9 +457,10 @@
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,8 +473,11 @@
       <c r="D1" t="s">
         <v>13</v>
       </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -474,8 +490,11 @@
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -488,8 +507,11 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -502,8 +524,16 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+      <formula1>"company coordinator, company as, company viewer"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>

</xml_diff>